<commit_message>
Optimized with new equation
- new model equation
- pretty good fit with residuals
</commit_message>
<xml_diff>
--- a/DataCollection/AllData_raw_csv/10mmParameters.xlsx
+++ b/DataCollection/AllData_raw_csv/10mmParameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\AllData_raw_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAF8491-067A-4E0F-8861-F129A6682240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04A79C0-2987-4C36-9018-349D43146E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{77D8A100-45DA-4248-AA11-EEE2BEBFD1BC}"/>
+    <workbookView xWindow="-24885" yWindow="1395" windowWidth="21600" windowHeight="11385" xr2:uid="{77D8A100-45DA-4248-AA11-EEE2BEBFD1BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Test10" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Data</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>(a2*strain)</t>
+  </si>
+  <si>
+    <t>Intercept</t>
   </si>
 </sst>
 </file>
@@ -316,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,6 +399,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2168,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401F6281-533D-4517-84CE-3CB45F536282}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2191,17 +2197,17 @@
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2213,17 +2219,17 @@
         <v>17</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="24" t="s">
+      <c r="J3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="24"/>
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="24"/>
+      <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2248,26 +2254,32 @@
       <c r="H4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="N4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="O4" s="20" t="s">
         <v>21</v>
       </c>
+      <c r="P4" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
@@ -2294,28 +2306,36 @@
         <f>D5*F5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="1">
+        <f>H5+E5</f>
+        <v>-59.043999999999997</v>
+      </c>
+      <c r="J5" s="3">
         <v>0.61463999999999996</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>-1837.9</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>-55.512999999999998</v>
       </c>
-      <c r="L5" s="10">
+      <c r="M5" s="10">
         <v>-52.014000000000003</v>
       </c>
-      <c r="M5" s="25">
-        <f>(I5+J5*F5)</f>
+      <c r="N5" s="25">
+        <f>(J5+K5*F5)</f>
         <v>0.61463999999999996</v>
       </c>
-      <c r="N5" s="20">
-        <f>K5*F5</f>
+      <c r="O5" s="20">
+        <f>L5*F5</f>
         <v>0</v>
       </c>
+      <c r="P5" s="1">
+        <f>M5+O5</f>
+        <v>-52.014000000000003</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="9">
         <v>-22.774000000000001</v>
@@ -2341,28 +2361,36 @@
         <f t="shared" ref="H6:H23" si="1">D6*F6</f>
         <v>-0.35833333333333361</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="29">
+        <f t="shared" ref="I6:I23" si="2">H6+E6</f>
+        <v>-130.72833333333332</v>
+      </c>
+      <c r="J6" s="3">
         <v>-1.7336</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>-69.917000000000002</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>8.2085000000000008</v>
       </c>
-      <c r="L6" s="10">
+      <c r="M6" s="10">
         <v>-105.97</v>
       </c>
-      <c r="M6" s="26">
-        <f t="shared" ref="M6:M23" si="2">(I6+J6*F6)</f>
+      <c r="N6" s="26">
+        <f>(J6+K6*F6)</f>
         <v>0.59696666666666864</v>
       </c>
-      <c r="N6" s="21">
-        <f t="shared" ref="N6:N23" si="3">K6*F6</f>
+      <c r="O6" s="21">
+        <f>L6*F6</f>
         <v>-0.2736166666666669</v>
       </c>
+      <c r="P6" s="29">
+        <f t="shared" ref="P6:P23" si="3">M6+O6</f>
+        <v>-106.24361666666667</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="9">
         <v>-15.079000000000001</v>
@@ -2388,28 +2416,36 @@
         <f t="shared" si="1"/>
         <v>0.813533333333334</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="29">
+        <f t="shared" si="2"/>
+        <v>-194.79646666666667</v>
+      </c>
+      <c r="J7" s="3">
         <v>-81.597999999999999</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <v>-1232.3</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>115.6</v>
       </c>
-      <c r="L7" s="10">
+      <c r="M7" s="10">
         <v>-157.94999999999999</v>
       </c>
-      <c r="M7" s="26">
-        <f t="shared" si="2"/>
+      <c r="N7" s="26">
+        <f>(J7+K7*F7)</f>
         <v>0.55533333333339385</v>
       </c>
-      <c r="N7" s="21">
+      <c r="O7" s="21">
+        <f>L7*F7</f>
+        <v>-7.7066666666666723</v>
+      </c>
+      <c r="P7" s="29">
         <f t="shared" si="3"/>
-        <v>-7.7066666666666723</v>
+        <v>-165.65666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="13">
         <v>-10.887</v>
@@ -2435,28 +2471,36 @@
         <f t="shared" si="1"/>
         <v>-23.858999999999984</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="29">
+        <f t="shared" si="2"/>
+        <v>-231.36899999999997</v>
+      </c>
+      <c r="J8" s="14">
         <v>-8.4231999999999996</v>
       </c>
-      <c r="J8" s="14">
+      <c r="K8" s="14">
         <v>-88.525999999999996</v>
       </c>
-      <c r="K8" s="14">
+      <c r="L8" s="14">
         <v>82.882999999999996</v>
       </c>
-      <c r="L8" s="15">
+      <c r="M8" s="15">
         <v>-153.41</v>
       </c>
-      <c r="M8" s="27">
-        <f t="shared" si="2"/>
+      <c r="N8" s="27">
+        <f>(J8+K8*F8)</f>
         <v>0.42939999999999401</v>
       </c>
-      <c r="N8" s="21">
+      <c r="O8" s="21">
+        <f>L8*F8</f>
+        <v>-8.2882999999999942</v>
+      </c>
+      <c r="P8" s="29">
         <f t="shared" si="3"/>
-        <v>-8.2882999999999942</v>
+        <v>-161.69829999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
@@ -2483,28 +2527,36 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="29">
+        <f t="shared" si="2"/>
+        <v>-58.101999999999997</v>
+      </c>
+      <c r="J9" s="17">
         <v>0.65929000000000004</v>
       </c>
-      <c r="J9" s="17">
+      <c r="K9" s="17">
         <v>-224.61</v>
       </c>
-      <c r="K9" s="17">
+      <c r="L9" s="17">
         <v>33.716000000000001</v>
       </c>
-      <c r="L9" s="18">
+      <c r="M9" s="18">
         <v>-48.645000000000003</v>
       </c>
-      <c r="M9" s="25">
-        <f t="shared" si="2"/>
+      <c r="N9" s="25">
+        <f>(J9+K9*F9)</f>
         <v>0.65929000000000004</v>
       </c>
-      <c r="N9" s="20">
+      <c r="O9" s="20">
+        <f>L9*F9</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-48.645000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="9">
         <v>-10.766</v>
@@ -2530,28 +2582,36 @@
         <f t="shared" si="1"/>
         <v>-9.2836363636363632</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="29">
+        <f t="shared" si="2"/>
+        <v>-269.3336363636364</v>
+      </c>
+      <c r="J10" s="3">
         <v>133.79</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>1953.2</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L10" s="3">
         <v>47.484000000000002</v>
       </c>
-      <c r="L10" s="10">
+      <c r="M10" s="10">
         <v>-219.31</v>
       </c>
-      <c r="M10" s="26">
-        <f t="shared" si="2"/>
+      <c r="N10" s="26">
+        <f>(J10+K10*F10)</f>
         <v>0.6172727272727343</v>
       </c>
-      <c r="N10" s="21">
+      <c r="O10" s="21">
+        <f>L10*F10</f>
+        <v>-3.2375454545454545</v>
+      </c>
+      <c r="P10" s="29">
         <f t="shared" si="3"/>
-        <v>-3.2375454545454545</v>
+        <v>-222.54754545454546</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="13">
         <v>34.57</v>
@@ -2577,28 +2637,36 @@
         <f t="shared" si="1"/>
         <v>-25.217090909090924</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="29">
+        <f t="shared" si="2"/>
+        <v>-336.84709090909092</v>
+      </c>
+      <c r="J11" s="14">
         <v>30.437999999999999</v>
       </c>
-      <c r="J11" s="14">
+      <c r="K11" s="14">
         <v>212.99</v>
       </c>
-      <c r="K11" s="14">
+      <c r="L11" s="14">
         <v>114.27</v>
       </c>
-      <c r="L11" s="15">
+      <c r="M11" s="15">
         <v>-207.53</v>
       </c>
-      <c r="M11" s="26">
-        <f t="shared" si="2"/>
+      <c r="N11" s="26">
+        <f>(J11+K11*F11)</f>
         <v>0.4257727272727081</v>
       </c>
-      <c r="N11" s="21">
+      <c r="O11" s="21">
+        <f>L11*F11</f>
+        <v>-16.101681818181827</v>
+      </c>
+      <c r="P11" s="29">
         <f t="shared" si="3"/>
-        <v>-16.101681818181827</v>
+        <v>-223.63168181818182</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>9</v>
       </c>
@@ -2626,28 +2694,36 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="29">
+        <f t="shared" si="2"/>
+        <v>-46.625</v>
+      </c>
+      <c r="J12" s="17">
         <v>0.63105</v>
       </c>
-      <c r="J12" s="17">
+      <c r="K12" s="17">
         <v>-832.77</v>
       </c>
-      <c r="K12" s="17">
+      <c r="L12" s="17">
         <v>-14.773999999999999</v>
       </c>
-      <c r="L12" s="18">
+      <c r="M12" s="18">
         <v>-27.236000000000001</v>
       </c>
-      <c r="M12" s="25">
-        <f t="shared" si="2"/>
+      <c r="N12" s="25">
+        <f>(J12+K12*F12)</f>
         <v>0.63105</v>
       </c>
-      <c r="N12" s="20">
+      <c r="O12" s="20">
+        <f>L12*F12</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-27.236000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9">
         <v>24.353000000000002</v>
@@ -2673,28 +2749,36 @@
         <f t="shared" si="1"/>
         <v>0.33964980544747048</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="29">
+        <f t="shared" si="2"/>
+        <v>-196.27035019455255</v>
+      </c>
+      <c r="J13" s="3">
         <v>-1.5601</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>-81.753</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L13" s="3">
         <v>-1.8831</v>
       </c>
-      <c r="L13" s="10">
+      <c r="M13" s="10">
         <v>-155.12</v>
       </c>
-      <c r="M13" s="26">
-        <f t="shared" si="2"/>
+      <c r="N13" s="26">
+        <f>(J13+K13*F13)</f>
         <v>0.66663540856030923</v>
       </c>
-      <c r="N13" s="21">
+      <c r="O13" s="21">
+        <f>L13*F13</f>
+        <v>5.1290661478599169E-2</v>
+      </c>
+      <c r="P13" s="29">
         <f t="shared" si="3"/>
-        <v>5.1290661478599169E-2</v>
+        <v>-155.06870933852142</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9">
         <v>94.668999999999997</v>
@@ -2720,28 +2804,36 @@
         <f t="shared" si="1"/>
         <v>-13.099027237354086</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="29">
+        <f t="shared" si="2"/>
+        <v>-244.33902723735409</v>
+      </c>
+      <c r="J14" s="3">
         <v>44.332000000000001</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>749.1</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>179.74</v>
       </c>
-      <c r="L14" s="10">
+      <c r="M14" s="10">
         <v>-180.05</v>
       </c>
-      <c r="M14" s="26">
-        <f t="shared" si="2"/>
+      <c r="N14" s="26">
+        <f>(J14+K14*F14)</f>
         <v>0.61021011673151548</v>
       </c>
-      <c r="N14" s="21">
+      <c r="O14" s="21">
+        <f>L14*F14</f>
+        <v>-10.490661478599222</v>
+      </c>
+      <c r="P14" s="29">
         <f t="shared" si="3"/>
-        <v>-10.490661478599222</v>
+        <v>-190.54066147859925</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="13">
         <v>84.567999999999998</v>
@@ -2767,28 +2859,36 @@
         <f t="shared" si="1"/>
         <v>-12.24922178988326</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="29">
+        <f t="shared" si="2"/>
+        <v>-298.52922178988325</v>
+      </c>
+      <c r="J15" s="14">
         <v>23.087</v>
       </c>
-      <c r="J15" s="14">
+      <c r="K15" s="14">
         <v>187.71</v>
       </c>
-      <c r="K15" s="14">
+      <c r="L15" s="14">
         <v>121.49</v>
       </c>
-      <c r="L15" s="15">
+      <c r="M15" s="15">
         <v>-195.19</v>
       </c>
-      <c r="M15" s="27">
-        <f t="shared" si="2"/>
+      <c r="N15" s="27">
+        <f>(J15+K15*F15)</f>
         <v>0.44493774319067469</v>
       </c>
-      <c r="N15" s="22">
+      <c r="O15" s="22">
+        <f>L15*F15</f>
+        <v>-14.654435797665359</v>
+      </c>
+      <c r="P15" s="29">
         <f t="shared" si="3"/>
-        <v>-14.654435797665359</v>
+        <v>-209.84443579766537</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>10</v>
       </c>
@@ -2816,28 +2916,36 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="29">
+        <f t="shared" si="2"/>
+        <v>-23.14</v>
+      </c>
+      <c r="J16" s="17">
         <v>0.66274999999999995</v>
       </c>
-      <c r="J16" s="17">
+      <c r="K16" s="17">
         <v>-38.064</v>
       </c>
-      <c r="K16" s="17">
+      <c r="L16" s="17">
         <v>4.5829000000000004</v>
       </c>
-      <c r="L16" s="18">
+      <c r="M16" s="18">
         <v>-10.651999999999999</v>
       </c>
-      <c r="M16" s="26">
-        <f t="shared" si="2"/>
+      <c r="N16" s="26">
+        <f>(J16+K16*F16)</f>
         <v>0.66274999999999995</v>
       </c>
-      <c r="N16" s="21">
+      <c r="O16" s="21">
+        <f>L16*F16</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-10.651999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9">
         <v>-81.838999999999999</v>
@@ -2863,28 +2971,36 @@
         <f t="shared" si="1"/>
         <v>1.2252099644128134</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="29">
+        <f t="shared" si="2"/>
+        <v>-230.5147900355872</v>
+      </c>
+      <c r="J17" s="3">
         <v>123.75</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <v>2034.6</v>
       </c>
-      <c r="K17" s="3">
+      <c r="L17" s="3">
         <v>52.276000000000003</v>
       </c>
-      <c r="L17" s="10">
+      <c r="M17" s="10">
         <v>-185.15</v>
       </c>
-      <c r="M17" s="26">
-        <f t="shared" si="2"/>
+      <c r="N17" s="26">
+        <f>(J17+K17*F17)</f>
         <v>0.6603202846973204</v>
       </c>
-      <c r="N17" s="21">
+      <c r="O17" s="21">
+        <f>L17*F17</f>
+        <v>-3.1626049822064108</v>
+      </c>
+      <c r="P17" s="29">
         <f t="shared" si="3"/>
-        <v>-3.1626049822064108</v>
+        <v>-188.31260498220641</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9">
         <v>140.78</v>
@@ -2910,28 +3026,36 @@
         <f t="shared" si="1"/>
         <v>-1.3688113879003563</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="29">
+        <f t="shared" si="2"/>
+        <v>-270.73881138790034</v>
+      </c>
+      <c r="J18" s="3">
         <v>55.841999999999999</v>
       </c>
-      <c r="J18" s="3">
+      <c r="K18" s="3">
         <v>555.13</v>
       </c>
-      <c r="K18" s="3">
+      <c r="L18" s="3">
         <v>211.96</v>
       </c>
-      <c r="L18" s="10">
+      <c r="M18" s="10">
         <v>-190.83</v>
       </c>
-      <c r="M18" s="26">
-        <f t="shared" si="2"/>
+      <c r="N18" s="26">
+        <f>(J18+K18*F18)</f>
         <v>0.52655516014233683</v>
       </c>
-      <c r="N18" s="21">
+      <c r="O18" s="21">
+        <f>L18*F18</f>
+        <v>-21.1205693950178</v>
+      </c>
+      <c r="P18" s="29">
         <f t="shared" si="3"/>
-        <v>-21.1205693950178</v>
+        <v>-211.95056939501782</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="13">
         <v>34.097000000000001</v>
@@ -2957,28 +3081,36 @@
         <f t="shared" si="1"/>
         <v>-27.861032028469754</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="29">
+        <f t="shared" si="2"/>
+        <v>-326.39103202846974</v>
+      </c>
+      <c r="J19" s="14">
         <v>24.933</v>
       </c>
-      <c r="J19" s="14">
+      <c r="K19" s="14">
         <v>168.28</v>
       </c>
-      <c r="K19" s="14">
+      <c r="L19" s="14">
         <v>108.43</v>
       </c>
-      <c r="L19" s="15">
+      <c r="M19" s="15">
         <v>-183.49</v>
       </c>
-      <c r="M19" s="27">
-        <f t="shared" si="2"/>
+      <c r="N19" s="27">
+        <f>(J19+K19*F19)</f>
         <v>0.37969039145906791</v>
       </c>
-      <c r="N19" s="22">
+      <c r="O19" s="22">
+        <f>L19*F19</f>
+        <v>-15.820747330960858</v>
+      </c>
+      <c r="P19" s="29">
         <f t="shared" si="3"/>
-        <v>-15.820747330960858</v>
+        <v>-199.31074733096088</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>11</v>
       </c>
@@ -3006,28 +3138,36 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="29">
+        <f t="shared" si="2"/>
+        <v>-38.988999999999997</v>
+      </c>
+      <c r="J20" s="17">
         <v>0.66181999999999996</v>
       </c>
-      <c r="J20" s="17">
+      <c r="K20" s="17">
         <v>-97.274000000000001</v>
       </c>
-      <c r="K20" s="17">
+      <c r="L20" s="17">
         <v>23.042999999999999</v>
       </c>
-      <c r="L20" s="18">
+      <c r="M20" s="18">
         <v>-25.815999999999999</v>
       </c>
-      <c r="M20" s="26">
-        <f t="shared" si="2"/>
+      <c r="N20" s="26">
+        <f>(J20+K20*F20)</f>
         <v>0.66181999999999996</v>
       </c>
-      <c r="N20" s="21">
+      <c r="O20" s="21">
+        <f>L20*F20</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-25.815999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -3055,28 +3195,36 @@
         <f t="shared" si="1"/>
         <v>-12.534661921708214</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="29">
+        <f t="shared" si="2"/>
+        <v>-243.64466192170823</v>
+      </c>
+      <c r="J21" s="3">
         <v>10.037000000000001</v>
       </c>
-      <c r="J21" s="3">
+      <c r="K21" s="3">
         <v>219.37</v>
       </c>
-      <c r="K21" s="3">
+      <c r="L21" s="3">
         <v>19.692</v>
       </c>
-      <c r="L21" s="10">
+      <c r="M21" s="10">
         <v>-193.79</v>
       </c>
-      <c r="M21" s="26">
-        <f t="shared" si="2"/>
+      <c r="N21" s="26">
+        <f>(J21+K21*F21)</f>
         <v>0.66888612099642053</v>
       </c>
-      <c r="N21" s="21">
+      <c r="O21" s="21">
+        <f>L21*F21</f>
+        <v>-0.84093950177936139</v>
+      </c>
+      <c r="P21" s="29">
         <f t="shared" si="3"/>
-        <v>-0.84093950177936139</v>
+        <v>-194.63093950177935</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="9">
         <v>246.87</v>
@@ -3102,28 +3250,36 @@
         <f t="shared" si="1"/>
         <v>-47.478505338078342</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="29">
+        <f t="shared" si="2"/>
+        <v>-280.41850533807832</v>
+      </c>
+      <c r="J22" s="3">
         <v>169.8</v>
       </c>
-      <c r="J22" s="3">
+      <c r="K22" s="3">
         <v>2160.9</v>
       </c>
-      <c r="K22" s="3">
+      <c r="L22" s="3">
         <v>201.06</v>
       </c>
-      <c r="L22" s="10">
+      <c r="M22" s="10">
         <v>-216.56</v>
       </c>
-      <c r="M22" s="26">
-        <f t="shared" si="2"/>
+      <c r="N22" s="26">
+        <f>(J22+K22*F22)</f>
         <v>0.61921708185033708</v>
       </c>
-      <c r="N22" s="21">
+      <c r="O22" s="21">
+        <f>L22*F22</f>
+        <v>-15.74135231316728</v>
+      </c>
+      <c r="P22" s="29">
         <f t="shared" si="3"/>
-        <v>-15.74135231316728</v>
+        <v>-232.30135231316729</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="13">
         <v>39.915999999999997</v>
@@ -3149,33 +3305,41 @@
         <f t="shared" si="1"/>
         <v>-17.937437722419933</v>
       </c>
-      <c r="I23" s="14">
+      <c r="I23" s="29">
+        <f t="shared" si="2"/>
+        <v>-309.5274377224199</v>
+      </c>
+      <c r="J23" s="14">
         <v>50.731999999999999</v>
       </c>
-      <c r="J23" s="14">
+      <c r="K23" s="14">
         <v>427.7</v>
       </c>
-      <c r="K23" s="14">
+      <c r="L23" s="14">
         <v>154.15</v>
       </c>
-      <c r="L23" s="15">
+      <c r="M23" s="15">
         <v>-217.14</v>
       </c>
-      <c r="M23" s="27">
-        <f t="shared" si="2"/>
+      <c r="N23" s="27">
+        <f>(J23+K23*F23)</f>
         <v>0.50388612099643382</v>
       </c>
-      <c r="N23" s="22">
+      <c r="O23" s="22">
+        <f>L23*F23</f>
+        <v>-18.103024911032033</v>
+      </c>
+      <c r="P23" s="29">
         <f t="shared" si="3"/>
-        <v>-18.103024911032033</v>
+        <v>-235.24302491103202</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E26" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E27" s="23" t="s">
         <v>20</v>
       </c>

</xml_diff>